<commit_message>
Commit in the begining of August
</commit_message>
<xml_diff>
--- a/experiments/programs/SeeDB_python/DiViz_airbnb/neighbourhood='Bronx'.xlsx
+++ b/experiments/programs/SeeDB_python/DiViz_airbnb/neighbourhood='Bronx'.xlsx
@@ -428,13 +428,10 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -461,7 +458,7 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>0.63781559205250316</v>
+        <v>0.64717166879980226</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -475,7 +472,7 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <v>0.57327307789703974</v>
+        <v>0.5728373335193182</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -489,21 +486,21 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>0.50332109761757149</v>
+        <v>0.50160225902261324</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5">
-        <v>0.46644911002143902</v>
+        <v>0.48693594073825253</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -511,27 +508,27 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6">
-        <v>0.43995606888028049</v>
+        <v>0.46770782053374299</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>0.37370152320976158</v>
+        <v>0.4536956034413292</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -539,13 +536,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8">
-        <v>0.35668383731706421</v>
+        <v>0.44128093957015779</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -553,27 +550,27 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
       </c>
       <c r="D9">
-        <v>0.34232286916557669</v>
+        <v>0.37179230335955099</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10">
-        <v>0.2667424846450569</v>
+        <v>0.3580731431574421</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -581,125 +578,125 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11">
-        <v>0.48765311326574767</v>
+        <v>0.35750414114615531</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12">
-        <v>0.35899684946468807</v>
+        <v>0.35674137603370237</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D13">
-        <v>0.35814390217728109</v>
+        <v>0.34010419525189389</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14">
-        <v>0.19529071736390199</v>
+        <v>0.30845320608883631</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15">
-        <v>0.14567172960806479</v>
+        <v>0.29497067402663468</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D16">
-        <v>0.1390743524419816</v>
+        <v>0.28403806221260802</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D17">
-        <v>0.13701020803417191</v>
+        <v>0.27021670692982053</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18">
-        <v>0.12652726768055711</v>
+        <v>0.26403532326756068</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
       </c>
       <c r="D19">
-        <v>4.2093270349409843E-2</v>
+        <v>0.24961759150527091</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -707,13 +704,13 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
       </c>
       <c r="D20">
-        <v>0.4536956034413292</v>
+        <v>0.2448236410280151</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -721,27 +718,27 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D21">
-        <v>0.3082141988048091</v>
+        <v>0.2132050820397299</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D22">
-        <v>0.29516742632489928</v>
+        <v>0.19529071736390199</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -749,89 +746,86 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
       </c>
       <c r="D23">
-        <v>0.28410952529404898</v>
+        <v>0.18771528810424681</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D24">
-        <v>0.27022102931026459</v>
+        <v>0.14567172960806479</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D25">
-        <v>0.2495453932356127</v>
+        <v>0.1390743524419816</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D26">
-        <v>0.2448236410280151</v>
+        <v>0.13747044018359539</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D27">
-        <v>0.2132050820397299</v>
+        <v>0.12645541200857971</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C28" t="s">
         <v>12</v>
       </c>
       <c r="D28">
-        <v>0.18776757598271149</v>
+        <v>4.2085676401330541E-2</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E37">
-    <sortCondition ref="A1"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>